<commit_message>
Se agrego columna fecha emitida en reporte de compra
</commit_message>
<xml_diff>
--- a/storage/CatalogoVehiculosGeneral.xlsx
+++ b/storage/CatalogoVehiculosGeneral.xlsx
@@ -1,31 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Programador\Downloads\CATALOGOS OPERADORES Y VEHICULOS CARTA PORTE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\nuevosistemapruebas\storage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{520398BF-C198-476B-A11D-8DEFCAB06C94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FA2C31B-4590-4CAB-BB48-BD7A2A93C1D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="33">
   <si>
     <t>Permiso de la SCT</t>
   </si>
@@ -61,9 +69,6 @@
   </si>
   <si>
     <t>NUG2598</t>
-  </si>
-  <si>
-    <t>CHEVROLET CAVALIER 2019</t>
   </si>
   <si>
     <t>Quálitas Compañía de Seguros, S.A. de C.V</t>
@@ -499,7 +504,7 @@
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -558,165 +563,165 @@
       <c r="E2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>12</v>
+      <c r="F2" s="1">
+        <v>2019</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="F3" s="1">
         <v>2016</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="F4" s="1">
         <v>2015</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D5" s="1">
         <v>950210401</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F5" s="1">
         <v>2021</v>
       </c>
       <c r="G5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="J5" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D6" s="1">
         <v>950215067</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F6" s="1">
         <v>2018</v>
       </c>
       <c r="G6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="H6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="J6" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F7" s="1">
         <v>2018</v>
       </c>
       <c r="G7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="H7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="J7" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -724,16 +729,16 @@
         <v>2016</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>